<commit_message>
add: Guardar porcentajes de utilizacion
</commit_message>
<xml_diff>
--- a/integrador/results.xlsx
+++ b/integrador/results.xlsx
@@ -60,7 +60,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:F151"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -82,1688 +82,3020 @@
           <t>practico promedio</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>psico utilizacion</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>teorico utilizacion</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>practico utilizacion</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>8.61223204885473</v>
+        <v>8.61668948425558</v>
       </c>
       <c r="B2" t="n">
-        <v>14.654827511874595</v>
+        <v>13.460168774209775</v>
       </c>
       <c r="C2" t="n">
-        <v>18.567123194683763</v>
+        <v>17.746226478608083</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.4741008661868891</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.15176333242029397</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.10449498604305175</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>8.61223204885473</v>
+        <v>8.513981853794803</v>
       </c>
       <c r="B3" t="n">
-        <v>14.654827511874595</v>
+        <v>14.793046366589957</v>
       </c>
       <c r="C3" t="n">
-        <v>18.567123194683763</v>
+        <v>18.51186274854336</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.46089128775849375</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.21762154646718176</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.14632885778863014</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8.64991367358197</v>
+        <v>8.205438692122334</v>
       </c>
       <c r="B4" t="n">
-        <v>14.718492681182102</v>
+        <v>15.813790317610954</v>
       </c>
       <c r="C4" t="n">
-        <v>18.18126440709356</v>
+        <v>16.888671061818055</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5194195805111825</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2050180744092131</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.08150186698533121</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8.94411146528074</v>
+        <v>8.088936050222845</v>
       </c>
       <c r="B5" t="n">
-        <v>12.128434257512435</v>
+        <v>14.97447942343735</v>
       </c>
       <c r="C5" t="n">
-        <v>19.312045438738703</v>
+        <v>18.689742760857857</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.46606811257144243</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2520771326202209</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.16364081644070747</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8.837776117686015</v>
+        <v>8.379427520159792</v>
       </c>
       <c r="B6" t="n">
-        <v>15.467790012872978</v>
+        <v>13.608292753184868</v>
       </c>
       <c r="C6" t="n">
-        <v>16.937658689824268</v>
+        <v>18.10051575993498</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.498929017965548</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.16889659057858253</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.14744402863687536</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>8.868648510574037</v>
+        <v>8.114064111422929</v>
       </c>
       <c r="B7" t="n">
-        <v>14.597336957248265</v>
+        <v>14.63356383323143</v>
       </c>
       <c r="C7" t="n">
-        <v>21.097104627902144</v>
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.3070487534050674</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.12462199555613498</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.06850293077289023</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8.300705887233992</v>
+        <v>8.495473442971388</v>
       </c>
       <c r="B8" t="n">
-        <v>13.353432929243722</v>
+        <v>14.752037979413283</v>
       </c>
       <c r="C8" t="n">
-        <v>18.304565639889468</v>
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.3668783010465998</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.14543779569519283</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.08485874260186843</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8.954563065675814</v>
+        <v>8.577804064347403</v>
       </c>
       <c r="B9" t="n">
-        <v>14.564771151376068</v>
+        <v>15.236929870622312</v>
       </c>
       <c r="C9" t="n">
-        <v>19.452442217050702</v>
+        <v>16.867705348723636</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.6173770677339399</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.23709920729391037</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.17240280288026918</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.023579751748125</v>
+        <v>8.744735676368453</v>
       </c>
       <c r="B10" t="n">
-        <v>11.804687791200905</v>
+        <v>12.38282468684481</v>
       </c>
       <c r="C10" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.3396073462030722</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.10796653917776913</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.09307067657091382</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>8.51339370295143</v>
+        <v>8.343587859540468</v>
       </c>
       <c r="B11" t="n">
-        <v>15.10028226782653</v>
+        <v>13.363160964022988</v>
       </c>
       <c r="C11" t="n">
-        <v>19.386848541181863</v>
+        <v>16.991047581886807</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.2993055141539453</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.11017905184480457</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0872074618434119</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9.315125083979371</v>
+        <v>9.33038107562598</v>
       </c>
       <c r="B12" t="n">
-        <v>15.025683092230752</v>
+        <v>12.650803460596642</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>20.05391205896501</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.6007804370714739</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.16971567474170784</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.14219118460704852</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8.181866980186314</v>
+        <v>8.012173938393335</v>
       </c>
       <c r="B13" t="n">
-        <v>13.399711080600696</v>
+        <v>14.612534027134643</v>
       </c>
       <c r="C13" t="n">
-        <v>17.564431970887835</v>
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.39369597866271416</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.19357121680525186</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.10370128509928012</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>8.520053165917538</v>
+        <v>8.008604396763623</v>
       </c>
       <c r="B14" t="n">
-        <v>17.994637502274063</v>
+        <v>14.176287498104072</v>
       </c>
       <c r="C14" t="n">
-        <v>20.388925326790773</v>
+        <v>22.31631432197018</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.4057712292333696</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.20791888330552635</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.12913523408892671</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>9.157772913622463</v>
+        <v>10.138637407011839</v>
       </c>
       <c r="B15" t="n">
-        <v>13.446267679096216</v>
+        <v>11.027087415307344</v>
       </c>
       <c r="C15" t="n">
-        <v>15.879790861219595</v>
+        <v>19.45730118702299</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.41211470232009473</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1062043645474107</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.11264494142049307</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>8.765217550593775</v>
+        <v>8.039739230062075</v>
       </c>
       <c r="B16" t="n">
-        <v>13.445153670204324</v>
+        <v>11.606212679931225</v>
       </c>
       <c r="C16" t="n">
-        <v>17.281820206403598</v>
+        <v>18.346239175169682</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.5931215027165276</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.2028703589963053</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.15520391356108462</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8.827572658447302</v>
+        <v>8.396361795387092</v>
       </c>
       <c r="B17" t="n">
-        <v>13.079990170847624</v>
+        <v>11.568633178698322</v>
       </c>
       <c r="C17" t="n">
-        <v>19.898765742416742</v>
+        <v>19.75500558382294</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.23509813027083853</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0722595082592977</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.04140394882110321</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>8.737243888435682</v>
+        <v>9.070148865180304</v>
       </c>
       <c r="B18" t="n">
-        <v>16.18359311728825</v>
+        <v>13.593090526434613</v>
       </c>
       <c r="C18" t="n">
-        <v>21.805432028644393</v>
+        <v>19.658411080621168</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.5036653094104343</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.1660998764734898</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.10405622480971434</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8.221223137116015</v>
+        <v>9.272183735489387</v>
       </c>
       <c r="B19" t="n">
-        <v>13.150943125916994</v>
+        <v>13.756250071203738</v>
       </c>
       <c r="C19" t="n">
-        <v>18.761513333260304</v>
+        <v>16.976768957767423</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.7694267921877592</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.2842720748780516</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.19554484863314062</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>9.134985581870383</v>
+        <v>9.36054570315248</v>
       </c>
       <c r="B20" t="n">
-        <v>14.880992443267017</v>
+        <v>13.975781990031596</v>
       </c>
       <c r="C20" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.36995161449645086</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.1577678800514042</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.06994019205666895</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>9.199131385794333</v>
+        <v>8.687188946187606</v>
       </c>
       <c r="B21" t="n">
-        <v>16.304634097598278</v>
+        <v>11.576717468284157</v>
       </c>
       <c r="C21" t="n">
-        <v>16.7000348509452</v>
+        <v>21.21974898271167</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.34254837708080244</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.11666618599998187</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.13672683293116486</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>8.422171041690705</v>
+        <v>8.20811574761863</v>
       </c>
       <c r="B22" t="n">
-        <v>12.646861702962191</v>
+        <v>14.775659571558238</v>
       </c>
       <c r="C22" t="n">
-        <v>17.900787033893703</v>
+        <v>19.663710231689265</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.48310838088799046</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.13427979510311105</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.11712526750707515</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>8.341213379727922</v>
+        <v>8.500292344097517</v>
       </c>
       <c r="B23" t="n">
-        <v>13.74767546836271</v>
+        <v>14.945099351092223</v>
       </c>
       <c r="C23" t="n">
-        <v>18.426686091223484</v>
+        <v>0.0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.47439995175161276</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.16703240380004286</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.051095038205184774</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>8.071840845113243</v>
+        <v>8.285627582760746</v>
       </c>
       <c r="B24" t="n">
-        <v>14.912295729207</v>
+        <v>13.494981740227034</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0</v>
+        <v>19.88002262116599</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.47712835307802803</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.1818707773563865</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.19930151054018022</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>8.340704586568684</v>
+        <v>8.727346513976164</v>
       </c>
       <c r="B25" t="n">
-        <v>14.201729662214408</v>
+        <v>12.39456752595461</v>
       </c>
       <c r="C25" t="n">
-        <v>21.373410943208945</v>
+        <v>20.124137864847555</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.6246424660698716</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.23119027865782388</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.22869845363406396</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9.117744488041195</v>
+        <v>8.359432224605504</v>
       </c>
       <c r="B26" t="n">
-        <v>12.710662917106761</v>
+        <v>11.081518171288447</v>
       </c>
       <c r="C26" t="n">
-        <v>17.091174986048983</v>
+        <v>13.823463762560836</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.43469047567948627</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.15762680023041256</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.14882503841055128</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>8.749006502745337</v>
+        <v>8.881240584256343</v>
       </c>
       <c r="B27" t="n">
-        <v>14.702906736251125</v>
+        <v>14.874806937306452</v>
       </c>
       <c r="C27" t="n">
-        <v>16.082757091884332</v>
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.2980284753016413</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.11477578905456416</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.06306337804676736</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>8.918160704087818</v>
+        <v>9.38826949771297</v>
       </c>
       <c r="B28" t="n">
-        <v>15.529174571830366</v>
+        <v>13.610289248820324</v>
       </c>
       <c r="C28" t="n">
-        <v>18.436829930599213</v>
+        <v>22.073962893383023</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.631433233832029</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.21507563643410174</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.13537307016229547</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>8.69311262870982</v>
+        <v>8.398748027566318</v>
       </c>
       <c r="B29" t="n">
-        <v>16.131036344827685</v>
+        <v>13.29238258658774</v>
       </c>
       <c r="C29" t="n">
-        <v>15.411600799417833</v>
+        <v>21.48831508465195</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.28294309706791887</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.11067418383205284</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.0813108023073398</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>8.305302690871605</v>
+        <v>9.669093267547373</v>
       </c>
       <c r="B30" t="n">
-        <v>16.2233677232336</v>
+        <v>13.032378656170716</v>
       </c>
       <c r="C30" t="n">
-        <v>18.89450346245133</v>
+        <v>17.59475741060454</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.5953034723691435</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.1871330530558857</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.17651109701510662</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>8.77660536434399</v>
+        <v>8.630298046629793</v>
       </c>
       <c r="B31" t="n">
-        <v>15.350718510884066</v>
+        <v>15.412845280166586</v>
       </c>
       <c r="C31" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.29348759578494904</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0597611109976135</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.02109120502593204</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>8.189659628872318</v>
+        <v>8.328141671858067</v>
       </c>
       <c r="B32" t="n">
-        <v>14.147996958183391</v>
+        <v>13.977519507860585</v>
       </c>
       <c r="C32" t="n">
-        <v>18.928946631970675</v>
+        <v>19.62465540510362</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.4560963667690066</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.15632528809448112</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.09459431294253512</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>8.813912992146175</v>
+        <v>7.83607710164607</v>
       </c>
       <c r="B33" t="n">
-        <v>15.388195328902835</v>
+        <v>14.10600363961091</v>
       </c>
       <c r="C33" t="n">
-        <v>17.383563534469406</v>
+        <v>14.551674537947756</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.3376358950034234</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.1316560339697018</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.12983594425334408</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>8.332567863987366</v>
+        <v>8.917867806736242</v>
       </c>
       <c r="B34" t="n">
-        <v>13.791368121615841</v>
+        <v>12.018292117618122</v>
       </c>
       <c r="C34" t="n">
-        <v>16.800896519446674</v>
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5567960814083537</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.17125642593035936</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.03277877504081957</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>8.42284694886182</v>
+        <v>8.557562225152532</v>
       </c>
       <c r="B35" t="n">
-        <v>16.059457371562985</v>
+        <v>12.855879790127386</v>
       </c>
       <c r="C35" t="n">
-        <v>17.50029278343326</v>
+        <v>18.516875095323137</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.4792234846085418</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.15886002355228604</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.10024921192059545</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>8.879530042785964</v>
+        <v>8.22298597633116</v>
       </c>
       <c r="B36" t="n">
-        <v>12.94888026377279</v>
+        <v>13.959634693480215</v>
       </c>
       <c r="C36" t="n">
-        <v>17.742239866214863</v>
+        <v>18.099202542151307</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.4607925088736935</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.20835841640809766</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.19548209400961544</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>8.658285944482069</v>
+        <v>9.185861129101536</v>
       </c>
       <c r="B37" t="n">
-        <v>16.8480482019022</v>
+        <v>16.84370523017126</v>
       </c>
       <c r="C37" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.48250960725354036</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.12936592672147873</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.008026831597810593</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>8.81679059797233</v>
+        <v>8.786964818155584</v>
       </c>
       <c r="B38" t="n">
-        <v>14.13092333847615</v>
+        <v>15.409795072078442</v>
       </c>
       <c r="C38" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.5239992292766511</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.16269952445753166</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.034218901015334015</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>8.129862979902587</v>
+        <v>9.064909730726187</v>
       </c>
       <c r="B39" t="n">
-        <v>12.793835126690805</v>
+        <v>13.617361102657265</v>
       </c>
       <c r="C39" t="n">
-        <v>17.416384426119627</v>
+        <v>16.94137546408583</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.6687889606040701</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.2688539346426952</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.175370527280439</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>8.840698679090396</v>
+        <v>9.769738268649071</v>
       </c>
       <c r="B40" t="n">
-        <v>17.229230305584327</v>
+        <v>11.888407885046824</v>
       </c>
       <c r="C40" t="n">
-        <v>17.35124926041546</v>
+        <v>15.520646608884409</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.4722921586182408</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.12997605598855155</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.054638294594341774</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>8.365086410430505</v>
+        <v>8.679286249134806</v>
       </c>
       <c r="B41" t="n">
-        <v>15.115204135983578</v>
+        <v>14.607833017781397</v>
       </c>
       <c r="C41" t="n">
-        <v>15.732837718001962</v>
+        <v>14.511904470068854</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.522409819128127</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.18724604656159258</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.10784868626021316</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>8.478752302176003</v>
+        <v>7.856232899831546</v>
       </c>
       <c r="B42" t="n">
-        <v>17.01025406193553</v>
+        <v>11.99488575462481</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0</v>
+        <v>18.09957993395176</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.3171564601429976</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.14316001950761265</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.07716181891080415</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>8.0397160748274</v>
+        <v>8.857060051750684</v>
       </c>
       <c r="B43" t="n">
-        <v>18.08650519954625</v>
+        <v>14.35738969945861</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0</v>
+        <v>24.468143233146552</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.3117240973206073</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.14620416422935992</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.09282334660838254</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>8.276346476420208</v>
+        <v>8.22542860327451</v>
       </c>
       <c r="B44" t="n">
-        <v>13.381240813039755</v>
+        <v>15.022461655413805</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0</v>
+        <v>16.43874324223682</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.4828239655813225</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.21412001938677838</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.09887241864003975</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>8.803506393276333</v>
+        <v>8.66313482953106</v>
       </c>
       <c r="B45" t="n">
-        <v>12.02260285262031</v>
+        <v>10.366237677153777</v>
       </c>
       <c r="C45" t="n">
-        <v>16.632578658044995</v>
+        <v>20.18575467218517</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5389985527855221</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.15670082713747974</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.14531169338600466</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>9.421741132513521</v>
+        <v>8.54587187768318</v>
       </c>
       <c r="B46" t="n">
-        <v>16.12839951844075</v>
+        <v>17.92631842234265</v>
       </c>
       <c r="C46" t="n">
-        <v>20.78413381867254</v>
+        <v>0.0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.5026304606878812</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.235525324737585</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.10111579221409588</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>9.0971978540831</v>
+        <v>8.333333697578462</v>
       </c>
       <c r="B47" t="n">
-        <v>14.116057480290985</v>
+        <v>13.381801036203992</v>
       </c>
       <c r="C47" t="n">
-        <v>17.922896804133085</v>
+        <v>0.0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.4204848791297294</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.16262481508822937</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.027060242899423492</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>8.095416081902234</v>
+        <v>8.044304151879045</v>
       </c>
       <c r="B48" t="n">
-        <v>16.160163688211743</v>
+        <v>13.523250508552685</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0</v>
+        <v>19.148995094761478</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.5363456096036818</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.1852250969706308</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.13501313102856363</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>9.075445889644168</v>
+        <v>8.26470409330901</v>
       </c>
       <c r="B49" t="n">
-        <v>14.610305416753507</v>
+        <v>14.442698680320184</v>
       </c>
       <c r="C49" t="n">
-        <v>18.280489917720104</v>
+        <v>16.938747419696416</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.4243284014863985</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.17779134631418533</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.1930455750544792</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>7.877380533617658</v>
+        <v>8.329621819413573</v>
       </c>
       <c r="B50" t="n">
-        <v>13.585229546728405</v>
+        <v>12.405278453058783</v>
       </c>
       <c r="C50" t="n">
-        <v>14.27187776370015</v>
+        <v>18.141737187106788</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.3539691730996205</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.07752391208640824</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.048009392130028854</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>9.136705481452747</v>
+        <v>7.9259045842124305</v>
       </c>
       <c r="B51" t="n">
-        <v>14.91929878181186</v>
+        <v>16.073846387888086</v>
       </c>
       <c r="C51" t="n">
-        <v>18.502577863988993</v>
+        <v>21.392218628149468</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.4346992042452199</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.16517545810408496</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.10125596695996981</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>8.483782042782186</v>
+        <v>8.71388874498321</v>
       </c>
       <c r="B52" t="n">
-        <v>14.92161183626527</v>
+        <v>14.075319015188304</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0</v>
+        <v>19.18364203473588</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.5993626998189229</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.20033705527844844</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.23696358666245562</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>10.078775176453279</v>
+        <v>8.63578077043392</v>
       </c>
       <c r="B53" t="n">
-        <v>15.78336995682652</v>
+        <v>15.112146317759665</v>
       </c>
       <c r="C53" t="n">
-        <v>20.113829135086927</v>
+        <v>13.969030530374944</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.507369875442546</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.19943181992440973</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.049611834083438715</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>8.010211900662425</v>
+        <v>8.053403280778854</v>
       </c>
       <c r="B54" t="n">
-        <v>14.25674572830921</v>
+        <v>14.671717482785377</v>
       </c>
       <c r="C54" t="n">
-        <v>17.21836515577131</v>
+        <v>22.807782232515976</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.5519108897701944</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.26503814279468685</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.19056181333342861</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>8.382298278033812</v>
+        <v>8.883205669362649</v>
       </c>
       <c r="B55" t="n">
-        <v>12.016134817593924</v>
+        <v>18.470380048449858</v>
       </c>
       <c r="C55" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.32819824228759226</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.17232118284710232</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.04865009491043188</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>7.720542050095145</v>
+        <v>8.405836151115857</v>
       </c>
       <c r="B56" t="n">
-        <v>14.892348574668935</v>
+        <v>12.302784413504732</v>
       </c>
       <c r="C56" t="n">
-        <v>21.876077368641337</v>
+        <v>20.48876404373817</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.43731152029237136</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.16061565608256387</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.12956750781583612</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>8.66504110590076</v>
+        <v>8.279221220409616</v>
       </c>
       <c r="B57" t="n">
-        <v>16.098800448623653</v>
+        <v>18.504286451970582</v>
       </c>
       <c r="C57" t="n">
-        <v>18.60560105276977</v>
+        <v>0.0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.23634029700264675</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.12438694442309507</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.04033514653636292</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>8.48679343371536</v>
+        <v>8.832833627880275</v>
       </c>
       <c r="B58" t="n">
-        <v>16.97910168333217</v>
+        <v>15.0342386162505</v>
       </c>
       <c r="C58" t="n">
-        <v>15.044545024872418</v>
+        <v>14.788489729593596</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.3961493279173949</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.14754944942039852</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.10734728958187112</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>9.73116151003415</v>
+        <v>8.41281378988695</v>
       </c>
       <c r="B59" t="n">
-        <v>13.810445546051664</v>
+        <v>13.101350749604165</v>
       </c>
       <c r="C59" t="n">
-        <v>16.97727604071977</v>
+        <v>19.667232304441267</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.5733846925150005</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.23907023568242364</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.24394299876440653</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>7.92462532535839</v>
+        <v>8.869945001074274</v>
       </c>
       <c r="B60" t="n">
-        <v>12.616809075493348</v>
+        <v>13.554993872652261</v>
       </c>
       <c r="C60" t="n">
-        <v>14.046510580887844</v>
+        <v>15.852229386770409</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.4377398683283841</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.16700519034867856</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.039034072949066335</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>8.648765010099075</v>
+        <v>8.747389852014788</v>
       </c>
       <c r="B61" t="n">
-        <v>12.77618276135507</v>
+        <v>14.472637215575892</v>
       </c>
       <c r="C61" t="n">
-        <v>20.73100408116029</v>
+        <v>0.0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.5876728832774277</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.20189935081642557</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.09736892851833519</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>8.15662703990843</v>
+        <v>9.175998282846283</v>
       </c>
       <c r="B62" t="n">
-        <v>14.764065328571824</v>
+        <v>13.704172153214687</v>
       </c>
       <c r="C62" t="n">
-        <v>16.707563444180277</v>
+        <v>17.024124776344262</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.4164552641322462</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.09642354561679481</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.05674708258781421</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>8.369979303495787</v>
+        <v>8.074145530131696</v>
       </c>
       <c r="B63" t="n">
-        <v>15.324777618722246</v>
+        <v>16.21388056703266</v>
       </c>
       <c r="C63" t="n">
-        <v>18.967205504625547</v>
+        <v>16.908746265409636</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.38952305971518675</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.19598019643840997</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0754248867201723</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>9.077511942559328</v>
+        <v>8.549681689353358</v>
       </c>
       <c r="B64" t="n">
-        <v>14.322320947944265</v>
+        <v>15.541384397520094</v>
       </c>
       <c r="C64" t="n">
-        <v>19.47932958272992</v>
+        <v>21.715700764216773</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.3863395574942164</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.09810182727017304</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.036192834607027956</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>8.161561661406521</v>
+        <v>8.607992401445179</v>
       </c>
       <c r="B65" t="n">
-        <v>14.914150621938377</v>
+        <v>16.48415866405697</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0</v>
+        <v>17.22825022998863</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.42094331937781854</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.14033867511802287</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.07351590792863295</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>8.047928728298617</v>
+        <v>8.679525219606596</v>
       </c>
       <c r="B66" t="n">
-        <v>11.971869557356113</v>
+        <v>15.24651191312473</v>
       </c>
       <c r="C66" t="n">
-        <v>20.134314778093017</v>
+        <v>17.31272892857656</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.5924361981638184</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.2592479286740784</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.19447963002709678</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>8.862327803419712</v>
+        <v>8.195108163913853</v>
       </c>
       <c r="B67" t="n">
-        <v>15.309792799763745</v>
+        <v>12.827114039051015</v>
       </c>
       <c r="C67" t="n">
-        <v>0.0</v>
+        <v>19.199921189292</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.5307461106535811</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.18954695621386256</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.09756753389373558</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>8.654891970633928</v>
+        <v>8.383925467904767</v>
       </c>
       <c r="B68" t="n">
-        <v>15.643926293557367</v>
+        <v>14.834095998393611</v>
       </c>
       <c r="C68" t="n">
-        <v>0.0</v>
+        <v>21.045847316442277</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.3773868234859346</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.13226867723744784</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.06984875540171732</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>8.239501590860122</v>
+        <v>9.151227214000393</v>
       </c>
       <c r="B69" t="n">
-        <v>14.975673560876457</v>
+        <v>14.51457953758884</v>
       </c>
       <c r="C69" t="n">
-        <v>17.021877129677115</v>
+        <v>19.01799297505419</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.7748752260965386</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.2768638947983561</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.1644278679304808</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>8.386963193889622</v>
+        <v>8.75072207107006</v>
       </c>
       <c r="B70" t="n">
-        <v>15.65683861231176</v>
+        <v>13.65755334334215</v>
       </c>
       <c r="C70" t="n">
-        <v>0.0</v>
+        <v>17.914540718378756</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.4844297162106642</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.20114819813912188</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.10399693237286563</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>8.857111640361076</v>
+        <v>8.389449801120547</v>
       </c>
       <c r="B71" t="n">
-        <v>13.276412735219186</v>
+        <v>14.506607555010548</v>
       </c>
       <c r="C71" t="n">
-        <v>17.839371615344287</v>
+        <v>0.0</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.43625138965826843</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.14159113028781503</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.09238053801324154</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>14.820779728663746</v>
+        <v>8.402078062545435</v>
       </c>
       <c r="B72" t="n">
-        <v>15.301955289428898</v>
+        <v>14.966950891901767</v>
       </c>
       <c r="C72" t="n">
-        <v>17.731529075026618</v>
+        <v>17.815336311488434</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.4838796193850269</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1847189614747271</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.1554749310932875</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>8.52314229050959</v>
+        <v>8.66992177559418</v>
       </c>
       <c r="B73" t="n">
-        <v>12.3500208726984</v>
+        <v>15.628089990323584</v>
       </c>
       <c r="C73" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.34029756277039125</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.14546578621409295</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.052819858960220234</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>8.568374331718983</v>
+        <v>8.663747313647978</v>
       </c>
       <c r="B74" t="n">
-        <v>13.23256395710086</v>
+        <v>13.698132023951596</v>
       </c>
       <c r="C74" t="n">
-        <v>18.696389649953357</v>
+        <v>0.0</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.28221987816410354</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.1425550263060114</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.04741201667922656</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>8.663002698057474</v>
+        <v>8.046999618272297</v>
       </c>
       <c r="B75" t="n">
-        <v>14.779313642426677</v>
+        <v>15.41910571818659</v>
       </c>
       <c r="C75" t="n">
-        <v>0.0</v>
+        <v>17.609643959945362</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.43287227781905513</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.23658637232737523</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.19474276403038204</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>9.219090591930533</v>
+        <v>8.019427289857301</v>
       </c>
       <c r="B76" t="n">
-        <v>12.681990338855318</v>
+        <v>17.077277596853698</v>
       </c>
       <c r="C76" t="n">
-        <v>15.95425884312179</v>
+        <v>17.250154715339523</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.4345447695807015</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.21221268942437552</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.11060199293586363</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>9.001699737203117</v>
+        <v>8.822242521186833</v>
       </c>
       <c r="B77" t="n">
-        <v>13.646279958335631</v>
+        <v>16.10856425671684</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0</v>
+        <v>19.127549128527907</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.5086078634559712</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.21174278807470073</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.1926123486063497</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>8.170215758000841</v>
+        <v>9.35402041236954</v>
       </c>
       <c r="B78" t="n">
-        <v>18.52472190698362</v>
+        <v>15.53631488197527</v>
       </c>
       <c r="C78" t="n">
-        <v>0.0</v>
+        <v>13.431385242457328</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.3814097979873373</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.1477992928094333</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.07300888746778893</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>8.5504875422441</v>
+        <v>8.566858690209406</v>
       </c>
       <c r="B79" t="n">
-        <v>15.464961246759175</v>
+        <v>14.23206905534292</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0</v>
+        <v>16.18856513778042</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.4575148004396805</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.1474688644590193</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0.11950156345722797</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>7.94797491699526</v>
+        <v>8.663699726531204</v>
       </c>
       <c r="B80" t="n">
-        <v>13.110839077378806</v>
+        <v>13.7444377747609</v>
       </c>
       <c r="C80" t="n">
-        <v>0.0</v>
+        <v>17.783059238106418</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.541146964930552</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.22528783221937637</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.1673257418225403</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>8.149244925005698</v>
+        <v>8.290113176065518</v>
       </c>
       <c r="B81" t="n">
-        <v>13.834155044581824</v>
+        <v>15.337047248946186</v>
       </c>
       <c r="C81" t="n">
-        <v>16.861868730821623</v>
+        <v>20.602260924426936</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.5753826402014093</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.24084383896214678</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.19726727231162924</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>8.345127766942593</v>
+        <v>8.407100547114812</v>
       </c>
       <c r="B82" t="n">
-        <v>17.07763345874514</v>
+        <v>11.711599125571343</v>
       </c>
       <c r="C82" t="n">
-        <v>0.0</v>
+        <v>18.433000957470963</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.2990627075499107</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.09924614113706705</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.12073591595704979</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>8.561257418777272</v>
+        <v>8.365117755797058</v>
       </c>
       <c r="B83" t="n">
-        <v>15.143119059728035</v>
+        <v>18.93455501142407</v>
       </c>
       <c r="C83" t="n">
-        <v>23.280002307691877</v>
+        <v>21.369456806359032</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.4052950224428019</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.19144931502274798</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.08216180220958409</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>8.620839952347584</v>
+        <v>9.108883470704107</v>
       </c>
       <c r="B84" t="n">
-        <v>14.037159952898522</v>
+        <v>14.358551187127558</v>
       </c>
       <c r="C84" t="n">
-        <v>22.49366678855957</v>
+        <v>13.925117981683346</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.48260166149031825</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.14487493255577097</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.08219670376158333</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>8.386318642411593</v>
+        <v>8.62654865260007</v>
       </c>
       <c r="B85" t="n">
-        <v>11.61845347506733</v>
+        <v>13.70327955941478</v>
       </c>
       <c r="C85" t="n">
-        <v>16.468252228536112</v>
+        <v>15.716667285817213</v>
+      </c>
+      <c r="D85" t="n">
+        <v>0.5630199432867894</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.1966325222072792</v>
+      </c>
+      <c r="F85" t="n">
+        <v>0.15267190894302668</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>8.573931343689948</v>
+        <v>8.792592617568152</v>
       </c>
       <c r="B86" t="n">
-        <v>16.595820718736167</v>
+        <v>17.76651496060015</v>
       </c>
       <c r="C86" t="n">
-        <v>19.882418836814566</v>
+        <v>17.44550072472098</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.4487875910155473</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.2152898578427098</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0.10889514797929682</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>8.597696626170784</v>
+        <v>8.884756619094228</v>
       </c>
       <c r="B87" t="n">
-        <v>14.073461672326312</v>
+        <v>13.21295103701902</v>
       </c>
       <c r="C87" t="n">
-        <v>0.0</v>
+        <v>22.06351624838754</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.4859236897529806</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.14288824903148603</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.11744463148551883</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>8.674683273838241</v>
+        <v>9.060214960213964</v>
       </c>
       <c r="B88" t="n">
-        <v>15.875814794751912</v>
+        <v>13.636323727656032</v>
       </c>
       <c r="C88" t="n">
-        <v>15.001643920030611</v>
+        <v>18.26622385187256</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.7463799308952769</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.31164707464491986</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.2324793496925066</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>8.5966922224917</v>
+        <v>7.857184007790156</v>
       </c>
       <c r="B89" t="n">
-        <v>10.270225881634044</v>
+        <v>17.896847255885337</v>
       </c>
       <c r="C89" t="n">
-        <v>19.27008261668909</v>
+        <v>17.098099646395173</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.3765906981018795</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.17672644972808305</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.09002287740022837</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>8.222311745208007</v>
+        <v>8.929992790184059</v>
       </c>
       <c r="B90" t="n">
-        <v>15.510574382463064</v>
+        <v>13.58023205378081</v>
       </c>
       <c r="C90" t="n">
-        <v>0.0</v>
+        <v>19.5563459182331</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.4226122286994521</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.13116385337747863</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.06476198769857434</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>8.130968298308355</v>
+        <v>8.592303053152998</v>
       </c>
       <c r="B91" t="n">
-        <v>17.423265870690976</v>
+        <v>14.444825845905035</v>
       </c>
       <c r="C91" t="n">
-        <v>0.0</v>
+        <v>16.468478973387008</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.5615351561094644</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.23441097463634689</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.15149952711637324</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>8.403790463889571</v>
+        <v>8.311190198543803</v>
       </c>
       <c r="B92" t="n">
-        <v>14.693740642083423</v>
+        <v>14.315478581694666</v>
       </c>
       <c r="C92" t="n">
-        <v>0.0</v>
+        <v>17.22257385718111</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.39893712953010263</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.1837766988124048</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.15391157712348177</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>8.304513346919155</v>
+        <v>8.580609651929832</v>
       </c>
       <c r="B93" t="n">
-        <v>13.377916357519622</v>
+        <v>12.382995300039703</v>
       </c>
       <c r="C93" t="n">
-        <v>18.714605563017606</v>
+        <v>19.005604243558714</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0.43328687045008457</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0.16466368135030518</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0.10656178342266016</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>8.74832700191567</v>
+        <v>8.450726577193096</v>
       </c>
       <c r="B94" t="n">
-        <v>17.81203764473428</v>
+        <v>17.17983443141539</v>
       </c>
       <c r="C94" t="n">
-        <v>0.0</v>
+        <v>16.00697898728124</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.3787706482721063</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.15464178627544378</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.038580034796287736</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>9.12113194577846</v>
+        <v>8.026658286981037</v>
       </c>
       <c r="B95" t="n">
-        <v>13.97139836071189</v>
+        <v>14.27294749584392</v>
       </c>
       <c r="C95" t="n">
-        <v>20.23605774166483</v>
+        <v>0.0</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.4541356553292516</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.1763247418405286</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.08463614575428839</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>9.146532197927465</v>
+        <v>8.144940948156403</v>
       </c>
       <c r="B96" t="n">
-        <v>11.57327357309721</v>
+        <v>15.663618235689626</v>
       </c>
       <c r="C96" t="n">
-        <v>19.838751223185717</v>
+        <v>18.71381996059995</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.3273900346239699</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.1153345437412489</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.06416043655698246</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>9.360088847274508</v>
+        <v>8.771945256970424</v>
       </c>
       <c r="B97" t="n">
-        <v>13.134843680394143</v>
+        <v>11.969499895371195</v>
       </c>
       <c r="C97" t="n">
-        <v>18.28340182121232</v>
+        <v>20.36366265418986</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.38834322801194227</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.090631269050108</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.07469549687694077</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>9.348717049462516</v>
+        <v>8.10855235133302</v>
       </c>
       <c r="B98" t="n">
-        <v>14.948942895649923</v>
+        <v>13.35672534787203</v>
       </c>
       <c r="C98" t="n">
-        <v>17.374368434987186</v>
+        <v>19.707530991675807</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.38822447197045407</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.15073993878994868</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.09959906558811928</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>8.12840191245093</v>
+        <v>7.896623112748855</v>
       </c>
       <c r="B99" t="n">
-        <v>14.167814571273372</v>
+        <v>15.625851406527357</v>
       </c>
       <c r="C99" t="n">
-        <v>17.513317055811658</v>
+        <v>20.076218267660927</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.492840303177479</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.2510700639836473</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.17650520941450185</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>8.844845486256354</v>
+        <v>8.491470313906989</v>
       </c>
       <c r="B100" t="n">
-        <v>18.775550624530812</v>
+        <v>13.449963990352698</v>
       </c>
       <c r="C100" t="n">
-        <v>19.396377308534365</v>
+        <v>20.42444582210628</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.6099325641348323</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0.21003025962743854</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0.1501805152743572</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>8.603569506080724</v>
+        <v>8.561568736081563</v>
       </c>
       <c r="B101" t="n">
-        <v>15.501152261732916</v>
+        <v>15.090861064575877</v>
       </c>
       <c r="C101" t="n">
-        <v>18.279238179343203</v>
+        <v>17.54197446475541</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.2874506357189238</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.1089789994175173</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.0679330747246767</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>8.14410083040735</v>
+        <v>9.53275753600261</v>
       </c>
       <c r="B102" t="n">
-        <v>15.029578382979453</v>
+        <v>16.929014045410245</v>
       </c>
       <c r="C102" t="n">
-        <v>22.22891693696601</v>
+        <v>0.0</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.6503716593499874</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.31417269757417926</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.06591466696586329</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>8.793494981872445</v>
+        <v>8.94896772137766</v>
       </c>
       <c r="B103" t="n">
-        <v>12.776497353121062</v>
+        <v>13.214903565721771</v>
       </c>
       <c r="C103" t="n">
-        <v>0.0</v>
+        <v>19.655451677450216</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.5082452368706455</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.17619871420962363</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.07714702213345027</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>8.712193613627546</v>
+        <v>8.785046741245395</v>
       </c>
       <c r="B104" t="n">
-        <v>13.835232235016129</v>
+        <v>14.796661964803118</v>
       </c>
       <c r="C104" t="n">
-        <v>20.517740967165928</v>
+        <v>17.45358122742335</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.5352104833187444</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.23797017781407273</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.17964324261141673</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>7.868731603777856</v>
+        <v>8.460716033156936</v>
       </c>
       <c r="B105" t="n">
-        <v>15.471030811939134</v>
+        <v>13.052095437645436</v>
       </c>
       <c r="C105" t="n">
-        <v>0.0</v>
+        <v>16.39489720055491</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.5161287629225028</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.19256841283788523</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.14229645576403904</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>8.30421256144388</v>
+        <v>8.999938338580394</v>
       </c>
       <c r="B106" t="n">
-        <v>14.514305457569575</v>
+        <v>14.495937235881994</v>
       </c>
       <c r="C106" t="n">
-        <v>16.533647432676332</v>
+        <v>18.999506479968733</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.32399778018889436</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.07780746615304772</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.031665844133281225</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>8.813183915405014</v>
+        <v>9.088666826322143</v>
       </c>
       <c r="B107" t="n">
-        <v>12.998540677054583</v>
+        <v>15.592702699048829</v>
       </c>
       <c r="C107" t="n">
-        <v>19.955448313258497</v>
+        <v>0.0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0.3271920057475971</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0.1449242613835142</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0.04564718324028999</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>8.566365603198125</v>
+        <v>9.47465537525435</v>
       </c>
       <c r="B108" t="n">
-        <v>13.915499039656716</v>
+        <v>12.627791969113671</v>
       </c>
       <c r="C108" t="n">
-        <v>20.179105094073464</v>
+        <v>18.35986290925115</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.5859856789723004</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.20264029966827588</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.1998922800191382</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>8.07218315729052</v>
+        <v>9.57578610027176</v>
       </c>
       <c r="B109" t="n">
-        <v>17.1041887016102</v>
+        <v>12.699318016293118</v>
       </c>
       <c r="C109" t="n">
-        <v>17.00174385776477</v>
+        <v>19.146358971736433</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.5712041880988133</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.27044518871844314</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.21893165650597732</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>8.305797258647523</v>
+        <v>7.834010147540058</v>
       </c>
       <c r="B110" t="n">
-        <v>12.49749823141292</v>
+        <v>16.69194129814822</v>
       </c>
       <c r="C110" t="n">
-        <v>18.477532857177714</v>
+        <v>0.0</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.2967727534858738</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.17142653626282303</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.13093734781269153</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>8.472855796201518</v>
+        <v>8.246138906818476</v>
       </c>
       <c r="B111" t="n">
-        <v>13.658960346527092</v>
+        <v>11.976551656195287</v>
       </c>
       <c r="C111" t="n">
-        <v>20.05528874242972</v>
+        <v>17.394738048604214</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.46178377878183463</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.15957716058925675</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.1519918209050878</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>8.737896408019719</v>
+        <v>8.355254533960693</v>
       </c>
       <c r="B112" t="n">
-        <v>14.773665638631396</v>
+        <v>16.526547324767584</v>
       </c>
       <c r="C112" t="n">
-        <v>16.382254601645737</v>
+        <v>17.30300801601064</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.5421585066325257</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.277634060133826</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.17352237830833703</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>7.868044153331575</v>
+        <v>8.967373019201185</v>
       </c>
       <c r="B113" t="n">
-        <v>14.318866242867607</v>
+        <v>16.167858190775323</v>
       </c>
       <c r="C113" t="n">
-        <v>19.103081029015307</v>
+        <v>18.0237249142281</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.5675855616652562</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.21953152222581776</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.07578199901591053</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>8.6178592894372</v>
+        <v>8.618966245500781</v>
       </c>
       <c r="B114" t="n">
-        <v>12.859740521578148</v>
+        <v>10.760777883141309</v>
       </c>
       <c r="C114" t="n">
-        <v>15.144040843718889</v>
+        <v>18.89031728098862</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0.37743243235482404</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0.09259590117796797</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0.0944515864049431</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>8.510994706468763</v>
+        <v>8.547176036315559</v>
       </c>
       <c r="B115" t="n">
-        <v>13.284698486496378</v>
+        <v>14.780573475820164</v>
       </c>
       <c r="C115" t="n">
-        <v>18.27084830229209</v>
+        <v>0.0</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.40942577692162707</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.17341877138603526</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.09137776161357514</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>9.274516534416588</v>
+        <v>8.042058818946352</v>
       </c>
       <c r="B116" t="n">
-        <v>10.832621759985509</v>
+        <v>15.91125340954338</v>
       </c>
       <c r="C116" t="n">
-        <v>18.819788244624284</v>
+        <v>19.179078542909036</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.23497480226693565</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.1224113469352091</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.09688433877781195</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>8.357105706842614</v>
+        <v>8.574530127561266</v>
       </c>
       <c r="B117" t="n">
-        <v>15.106675268859265</v>
+        <v>11.20808834457502</v>
       </c>
       <c r="C117" t="n">
-        <v>18.989919122531102</v>
+        <v>17.642882518967117</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.6573898421339051</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.19862065807198095</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.1698037569363283</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>8.914965470006429</v>
+        <v>8.21245897423138</v>
       </c>
       <c r="B118" t="n">
-        <v>16.151455536218727</v>
+        <v>16.59342871545544</v>
       </c>
       <c r="C118" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.3284983589692553</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.1754291705046825</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.05501502864743631</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>9.262904896420924</v>
+        <v>8.159976303600308</v>
       </c>
       <c r="B119" t="n">
-        <v>18.205399606811223</v>
+        <v>12.492576946869045</v>
       </c>
       <c r="C119" t="n">
-        <v>0.0</v>
+        <v>19.77535092429665</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.31671508953800903</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.08922095852220312</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.0631812056021879</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>8.747625876244397</v>
+        <v>8.48991514579387</v>
       </c>
       <c r="B120" t="n">
-        <v>16.95774187888982</v>
+        <v>11.796619573027387</v>
       </c>
       <c r="C120" t="n">
-        <v>21.46476748374422</v>
+        <v>0.0</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.5710767359349253</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.14511338989712697</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.08965103551271658</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>8.34784462409662</v>
+        <v>8.761980277641754</v>
       </c>
       <c r="B121" t="n">
-        <v>16.292499755205743</v>
+        <v>15.30368738395232</v>
       </c>
       <c r="C121" t="n">
-        <v>0.0</v>
+        <v>16.255165656025373</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.5126688315158896</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0.23336288478699105</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0.09912332841037541</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>8.678730627507882</v>
+        <v>8.280124746871866</v>
       </c>
       <c r="B122" t="n">
-        <v>14.30106185712921</v>
+        <v>14.543341102675829</v>
       </c>
       <c r="C122" t="n">
-        <v>17.301297726459925</v>
+        <v>18.88571689940259</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.3920176195513877</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.1405982534487488</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.09862003464700042</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>8.444629289925993</v>
+        <v>8.447612265159348</v>
       </c>
       <c r="B123" t="n">
-        <v>16.18620190432275</v>
+        <v>15.710497133067731</v>
       </c>
       <c r="C123" t="n">
-        <v>0.0</v>
+        <v>18.044805590932658</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.5421473423798471</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.26332267303070545</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.13326433742254812</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>8.192887211909246</v>
+        <v>8.174797672777343</v>
       </c>
       <c r="B124" t="n">
-        <v>16.151568126333597</v>
+        <v>15.644704645680173</v>
       </c>
       <c r="C124" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.3378130711022552</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.17510580842225004</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.028561659598906376</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>8.454329238885427</v>
+        <v>8.254033882990093</v>
       </c>
       <c r="B125" t="n">
-        <v>12.867219757667844</v>
+        <v>14.382658297279878</v>
       </c>
       <c r="C125" t="n">
-        <v>19.706339305647216</v>
+        <v>0.0</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.3775267003195646</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.12972252691540961</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.032735296811047594</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>8.45659855724241</v>
+        <v>8.320807579846724</v>
       </c>
       <c r="B126" t="n">
-        <v>15.367031897823502</v>
+        <v>14.030176731662985</v>
       </c>
       <c r="C126" t="n">
-        <v>19.853033625762468</v>
+        <v>15.923988371341734</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.3972145654297926</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.1988662040784758</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.1627970719501764</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>8.332187220429127</v>
+        <v>9.089512235980822</v>
       </c>
       <c r="B127" t="n">
-        <v>14.856109947599816</v>
+        <v>13.604217265731295</v>
       </c>
       <c r="C127" t="n">
-        <v>19.19142375400644</v>
+        <v>19.392030417842005</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.5749138231031894</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.20042217874896695</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.17697186614372348</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>8.474390559198776</v>
+        <v>8.731758465654442</v>
       </c>
       <c r="B128" t="n">
-        <v>12.536703741874815</v>
+        <v>15.458498389535002</v>
       </c>
       <c r="C128" t="n">
-        <v>17.503239238922895</v>
+        <v>0.0</v>
+      </c>
+      <c r="D128" t="n">
+        <v>0.3950004907560801</v>
+      </c>
+      <c r="E128" t="n">
+        <v>0.17525096132131399</v>
+      </c>
+      <c r="F128" t="n">
+        <v>0.12256832930933166</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>8.769753356538741</v>
+        <v>8.687749862854755</v>
       </c>
       <c r="B129" t="n">
-        <v>16.18627319068328</v>
+        <v>14.535870669909945</v>
       </c>
       <c r="C129" t="n">
-        <v>19.28325930418335</v>
+        <v>18.448660161712876</v>
+      </c>
+      <c r="D129" t="n">
+        <v>0.48068642525817024</v>
+      </c>
+      <c r="E129" t="n">
+        <v>0.18541459944493704</v>
+      </c>
+      <c r="F129" t="n">
+        <v>0.13265268522485815</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>8.550148852852665</v>
+        <v>8.38485780111726</v>
       </c>
       <c r="B130" t="n">
-        <v>12.243984175852688</v>
+        <v>13.93973208543463</v>
       </c>
       <c r="C130" t="n">
-        <v>19.75576316947229</v>
+        <v>16.298353867614527</v>
+      </c>
+      <c r="D130" t="n">
+        <v>0.5788456360781621</v>
+      </c>
+      <c r="E130" t="n">
+        <v>0.28334394229363435</v>
+      </c>
+      <c r="F130" t="n">
+        <v>0.21571745069664572</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>8.563581994700899</v>
+        <v>8.537285373445604</v>
       </c>
       <c r="B131" t="n">
-        <v>16.642132608444324</v>
+        <v>15.306759304285775</v>
       </c>
       <c r="C131" t="n">
-        <v>0.0</v>
+        <v>18.37712524074441</v>
+      </c>
+      <c r="D131" t="n">
+        <v>0.7674552581493649</v>
+      </c>
+      <c r="E131" t="n">
+        <v>0.29245145391867167</v>
+      </c>
+      <c r="F131" t="n">
+        <v>0.202244507264184</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>8.966952782048885</v>
+        <v>7.953179183110361</v>
       </c>
       <c r="B132" t="n">
-        <v>14.558582920668698</v>
+        <v>13.952034125948407</v>
       </c>
       <c r="C132" t="n">
-        <v>17.971735657898375</v>
+        <v>17.164083270801893</v>
+      </c>
+      <c r="D132" t="n">
+        <v>0.36133249481370094</v>
+      </c>
+      <c r="E132" t="n">
+        <v>0.16290076816001656</v>
+      </c>
+      <c r="F132" t="n">
+        <v>0.12239842665911155</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>8.941290951357873</v>
+        <v>8.034242514341383</v>
       </c>
       <c r="B133" t="n">
-        <v>14.115707311632576</v>
+        <v>13.675846703789727</v>
       </c>
       <c r="C133" t="n">
-        <v>19.180382868478034</v>
+        <v>19.172339728935672</v>
+      </c>
+      <c r="D133" t="n">
+        <v>0.5238902854189922</v>
+      </c>
+      <c r="E133" t="n">
+        <v>0.21317498324567888</v>
+      </c>
+      <c r="F133" t="n">
+        <v>0.15428252827976496</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>7.950995689302794</v>
+        <v>8.464686831692678</v>
       </c>
       <c r="B134" t="n">
-        <v>14.551432895253035</v>
+        <v>19.451422851359673</v>
       </c>
       <c r="C134" t="n">
-        <v>16.838660513636228</v>
+        <v>0.0</v>
+      </c>
+      <c r="D134" t="n">
+        <v>0.37908092914524205</v>
+      </c>
+      <c r="E134" t="n">
+        <v>0.11666955059785956</v>
+      </c>
+      <c r="F134" t="n">
+        <v>0.04427376617313144</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>8.971616208677151</v>
+        <v>8.198428803545575</v>
       </c>
       <c r="B135" t="n">
-        <v>14.248423207944303</v>
+        <v>14.351916844394681</v>
       </c>
       <c r="C135" t="n">
-        <v>0.0</v>
+        <v>16.24354030027731</v>
+      </c>
+      <c r="D135" t="n">
+        <v>0.29521645868808466</v>
+      </c>
+      <c r="E135" t="n">
+        <v>0.12793264724832726</v>
+      </c>
+      <c r="F135" t="n">
+        <v>0.08530006974078004</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>8.737358559185829</v>
+        <v>8.624962514308708</v>
       </c>
       <c r="B136" t="n">
-        <v>13.725742272074303</v>
+        <v>14.825325931076238</v>
       </c>
       <c r="C136" t="n">
-        <v>17.411318703726465</v>
+        <v>23.242172950690154</v>
+      </c>
+      <c r="D136" t="n">
+        <v>0.44794065150370993</v>
+      </c>
+      <c r="E136" t="n">
+        <v>0.18926148212082636</v>
+      </c>
+      <c r="F136" t="n">
+        <v>0.10122370881486593</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>8.558853285807455</v>
+        <v>8.651988343790089</v>
       </c>
       <c r="B137" t="n">
-        <v>16.212043196645478</v>
+        <v>13.616358914183015</v>
       </c>
       <c r="C137" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D137" t="n">
+        <v>0.3460795337516035</v>
+      </c>
+      <c r="E137" t="n">
+        <v>0.14774733296722084</v>
+      </c>
+      <c r="F137" t="n">
+        <v>0.062337993852516545</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>8.192114176095355</v>
+        <v>8.647043694119633</v>
       </c>
       <c r="B138" t="n">
-        <v>15.359819092178101</v>
+        <v>15.78957465757668</v>
       </c>
       <c r="C138" t="n">
-        <v>21.368894628325105</v>
+        <v>16.132906944023087</v>
+      </c>
+      <c r="D138" t="n">
+        <v>0.5650838624265828</v>
+      </c>
+      <c r="E138" t="n">
+        <v>0.2549252486047634</v>
+      </c>
+      <c r="F138" t="n">
+        <v>0.11630784778907723</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>9.110289359677656</v>
+        <v>8.98116993972376</v>
       </c>
       <c r="B139" t="n">
-        <v>14.151926171093628</v>
+        <v>13.025480991171074</v>
       </c>
       <c r="C139" t="n">
-        <v>18.11990800636049</v>
+        <v>22.115017634495455</v>
+      </c>
+      <c r="D139" t="n">
+        <v>0.4315727953975002</v>
+      </c>
+      <c r="E139" t="n">
+        <v>0.14408026677221725</v>
+      </c>
+      <c r="F139" t="n">
+        <v>0.14957187599113728</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>8.204863155945567</v>
+        <v>8.20911528647132</v>
       </c>
       <c r="B140" t="n">
-        <v>13.525119719729426</v>
+        <v>13.397280159666183</v>
       </c>
       <c r="C140" t="n">
-        <v>18.624615797408417</v>
+        <v>15.973643732087007</v>
+      </c>
+      <c r="D140" t="n">
+        <v>0.39403753375062334</v>
+      </c>
+      <c r="E140" t="n">
+        <v>0.13998677106159382</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0.10112032784074408</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>9.299732689029977</v>
+        <v>10.667698531071377</v>
       </c>
       <c r="B141" t="n">
-        <v>13.084722128950562</v>
+        <v>12.661245521887832</v>
       </c>
       <c r="C141" t="n">
-        <v>19.634849485684622</v>
+        <v>16.95385135820195</v>
+      </c>
+      <c r="D141" t="n">
+        <v>0.7794148238585411</v>
+      </c>
+      <c r="E141" t="n">
+        <v>0.25680758779112467</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0.1761044457245323</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>8.444106065171223</v>
+        <v>9.83299422822565</v>
       </c>
       <c r="B142" t="n">
-        <v>14.223159998824888</v>
+        <v>13.02491777226288</v>
       </c>
       <c r="C142" t="n">
-        <v>17.12834862967521</v>
+        <v>15.250515942693808</v>
+      </c>
+      <c r="D142" t="n">
+        <v>0.6850278278637619</v>
+      </c>
+      <c r="E142" t="n">
+        <v>0.25943723591897716</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0.1841453455023654</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>11.796426493267345</v>
+        <v>8.3131833579891</v>
       </c>
       <c r="B143" t="n">
-        <v>14.137536903117718</v>
+        <v>12.588221235090566</v>
       </c>
       <c r="C143" t="n">
         <v>0.0</v>
+      </c>
+      <c r="D143" t="n">
+        <v>0.42102175204403014</v>
+      </c>
+      <c r="E143" t="n">
+        <v>0.1583443230649299</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0.059961216319254364</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>9.148568865780044</v>
+        <v>8.985498524897643</v>
       </c>
       <c r="B144" t="n">
-        <v>13.152762182061805</v>
+        <v>14.69972496728081</v>
       </c>
       <c r="C144" t="n">
-        <v>14.881680862262519</v>
+        <v>19.153088997069954</v>
+      </c>
+      <c r="D144" t="n">
+        <v>0.43462806959892103</v>
+      </c>
+      <c r="E144" t="n">
+        <v>0.19122321638229647</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0.159470096724853</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>8.216171856642905</v>
+        <v>8.733736281176395</v>
       </c>
       <c r="B145" t="n">
-        <v>12.304006477337891</v>
+        <v>11.899171915274534</v>
       </c>
       <c r="C145" t="n">
-        <v>18.34061129036451</v>
+        <v>16.23973075715814</v>
+      </c>
+      <c r="D145" t="n">
+        <v>0.42463703129153296</v>
+      </c>
+      <c r="E145" t="n">
+        <v>0.14820156120276765</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0.08408157761341613</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>8.727591863141326</v>
+        <v>8.124424508777674</v>
       </c>
       <c r="B146" t="n">
-        <v>14.685417760840242</v>
+        <v>15.259898088363903</v>
       </c>
       <c r="C146" t="n">
-        <v>16.306802337382546</v>
+        <v>17.20788294957659</v>
+      </c>
+      <c r="D146" t="n">
+        <v>0.42314099704449737</v>
+      </c>
+      <c r="E146" t="n">
+        <v>0.1538954036768891</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0.14077355713063172</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>8.787364820343265</v>
+        <v>8.545595988221448</v>
       </c>
       <c r="B147" t="n">
-        <v>13.852870001320307</v>
+        <v>15.895431811378037</v>
       </c>
       <c r="C147" t="n">
-        <v>18.27722600743241</v>
+        <v>16.635704732772567</v>
+      </c>
+      <c r="D147" t="n">
+        <v>0.26162175449333086</v>
+      </c>
+      <c r="E147" t="n">
+        <v>0.10652795741788222</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0.07916037975984096</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>8.212259959372195</v>
+        <v>8.63656892414661</v>
       </c>
       <c r="B148" t="n">
-        <v>16.82462696246529</v>
+        <v>14.716740803187093</v>
       </c>
       <c r="C148" t="n">
-        <v>0.0</v>
+        <v>20.777797090148017</v>
+      </c>
+      <c r="D148" t="n">
+        <v>0.34842818424436406</v>
+      </c>
+      <c r="E148" t="n">
+        <v>0.17906848172425874</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0.07520174009609167</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>8.63335590126489</v>
+        <v>7.797294806930647</v>
       </c>
       <c r="B149" t="n">
-        <v>17.737137947414126</v>
+        <v>14.535320958684682</v>
       </c>
       <c r="C149" t="n">
-        <v>0.0</v>
+        <v>19.916414449824078</v>
+      </c>
+      <c r="D149" t="n">
+        <v>0.3265583326073934</v>
+      </c>
+      <c r="E149" t="n">
+        <v>0.13924625506623653</v>
+      </c>
+      <c r="F149" t="n">
+        <v>0.10599917558604573</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>9.108008074013245</v>
+        <v>8.804221496153307</v>
       </c>
       <c r="B150" t="n">
-        <v>16.214023646253892</v>
+        <v>13.75531671296094</v>
       </c>
       <c r="C150" t="n">
-        <v>0.0</v>
+        <v>18.198332198277466</v>
+      </c>
+      <c r="D150" t="n">
+        <v>0.6960896534846903</v>
+      </c>
+      <c r="E150" t="n">
+        <v>0.28381085371777576</v>
+      </c>
+      <c r="F150" t="n">
+        <v>0.12475796602755303</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>8.830189455532091</v>
+        <v>9.119779840385503</v>
       </c>
       <c r="B151" t="n">
-        <v>15.613482746123077</v>
+        <v>13.597522850854096</v>
       </c>
       <c r="C151" t="n">
-        <v>18.02425023744021</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="n">
-        <v>8.3351820925435</v>
-      </c>
-      <c r="B152" t="n">
-        <v>16.72844579948987</v>
-      </c>
-      <c r="C152" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="n">
-        <v>8.407314377831812</v>
-      </c>
-      <c r="B153" t="n">
-        <v>16.74776541303842</v>
-      </c>
-      <c r="C153" t="n">
-        <v>16.38956231383661</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="n">
-        <v>8.885787582978756</v>
-      </c>
-      <c r="B154" t="n">
-        <v>16.323441701285027</v>
-      </c>
-      <c r="C154" t="n">
-        <v>15.310028615626086</v>
+        <v>0.0</v>
+      </c>
+      <c r="D151" t="n">
+        <v>0.36299564974329723</v>
+      </c>
+      <c r="E151" t="n">
+        <v>0.16317027421024918</v>
+      </c>
+      <c r="F151" t="n">
+        <v>0.09394106954938951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>